<commit_message>
general: - add the icon - report on the failed contacts in the summary - trim the template column while generating - reset the lookups on Go - tell the user that the csv file is open
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Version</t>
   </si>
@@ -29,6 +29,14 @@
   </si>
   <si>
     <t>~ general infrastructure</t>
+  </si>
+  <si>
+    <t>general:
+- add the icon
+- report on the failed contacts in the summary
+- trim the template column while generating
+- reset the lookups on Go
+- tell the user that the csv file is open</t>
   </si>
 </sst>
 </file>
@@ -64,9 +72,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,8 +127,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="0"/>
     <tableColumn id="2" name="Comments"/>
@@ -170,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +457,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
[1.3] ~ print in the middle of the envelop Address1 in its first line and Address2 in the second line ~ give the user the option to generate for each contact: the letter only or envelop only or both
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Version</t>
   </si>
@@ -37,6 +38,28 @@
 - trim the template column while generating
 - reset the lookups on Go
 - tell the user that the csv file is open</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>~ add the option to print the envelope and/or the letter</t>
+  </si>
+  <si>
+    <t>add a print button for the tool to go over all of the generated documents and print them</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>[1.3]</t>
+  </si>
+  <si>
+    <t>~ print in the middle of the envelop Address1 in its first line and Address2 in the second line
+~ give the user the option to generate for each contact: the letter only or envelop only or both</t>
   </si>
 </sst>
 </file>
@@ -127,14 +150,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="0"/>
     <tableColumn id="2" name="Comments"/>
     <tableColumn id="3" name="Released"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Version"/>
+    <tableColumn id="2" name="Details"/>
+    <tableColumn id="3" name="Date"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -181,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,7 +251,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -425,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,11 +493,66 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.1000000000000001</v>
+      <c r="A3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="83.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a print button - still needs testing on Gerson's site
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Version</t>
   </si>
@@ -60,6 +60,9 @@
   <si>
     <t>~ print in the middle of the envelop Address1 in its first line and Address2 in the second line
 ~ give the user the option to generate for each contact: the letter only or envelop only or both</t>
+  </si>
+  <si>
+    <t>[1.4]</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +554,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
[1.5] add Address (FSAdress) field to the templates and csv and code
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Version</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>[1.4]</t>
+  </si>
+  <si>
+    <t>[1.5]</t>
+  </si>
+  <si>
+    <t>add FSAddress field to the templates and csv and code</t>
   </si>
 </sst>
 </file>
@@ -98,12 +104,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,8 +172,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version"/>
     <tableColumn id="2" name="Details"/>
@@ -521,10 +528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,6 +568,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
[1.6] ~ for each contact generate a filled copy of the envelop for each address set ~ for each contact generate carbon copies of the letter if the contact has more than one address set
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Version</t>
   </si>
@@ -69,6 +69,13 @@
   </si>
   <si>
     <t>add FSAddress field to the templates and csv and code</t>
+  </si>
+  <si>
+    <t>~ for each contact generate a filled copy of the envelop for each address set
+~ for each contact generate carbon copies of the letter if the contact has more than one address set</t>
+  </si>
+  <si>
+    <t>[1.6]</t>
   </si>
 </sst>
 </file>
@@ -172,8 +179,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version"/>
     <tableColumn id="2" name="Details"/>
@@ -528,10 +535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +586,17 @@
         <v>43222</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
fix a bug which prevented FsAddress field from being generated
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -75,7 +75,7 @@
 ~ for each contact generate carbon copies of the letter if the contact has more than one address set</t>
   </si>
   <si>
-    <t>[1.6]</t>
+    <t>[1.7]</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A5:C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[1.9] - use the new csv format and map Apptivo template name to CDMailer template name - fix: prompt for input csv incorrect - zipCode: insert leading 0 if it is less than 5
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,32 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Released</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>~ general infrastructure</t>
@@ -40,12 +31,6 @@
 - tell the user that the csv file is open</t>
   </si>
   <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>~ add the option to print the envelope and/or the letter</t>
-  </si>
-  <si>
     <t>add a print button for the tool to go over all of the generated documents and print them</t>
   </si>
   <si>
@@ -56,10 +41,6 @@
   </si>
   <si>
     <t>[1.3]</t>
-  </si>
-  <si>
-    <t>~ print in the middle of the envelop Address1 in its first line and Address2 in the second line
-~ give the user the option to generate for each contact: the letter only or envelop only or both</t>
   </si>
   <si>
     <t>[1.4]</t>
@@ -76,6 +57,316 @@
   </si>
   <si>
     <t>[1.7]</t>
+  </si>
+  <si>
+    <t>[1.8]</t>
+  </si>
+  <si>
+    <t>removing bad chars</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Opp Name</t>
+  </si>
+  <si>
+    <t>Fs Address</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>A1 - Address Line1</t>
+  </si>
+  <si>
+    <t>A1 - Address Line2</t>
+  </si>
+  <si>
+    <t>A1 - City</t>
+  </si>
+  <si>
+    <t>A1 - State</t>
+  </si>
+  <si>
+    <t>A1 - Zip Code</t>
+  </si>
+  <si>
+    <t>A2 - Address Line1</t>
+  </si>
+  <si>
+    <t>A2 - Address Line2</t>
+  </si>
+  <si>
+    <t>A2 - City</t>
+  </si>
+  <si>
+    <t>A2 - State</t>
+  </si>
+  <si>
+    <t>A2 - Zip Code</t>
+  </si>
+  <si>
+    <t>A3 - Address Line1</t>
+  </si>
+  <si>
+    <t>A3 - Address Line2</t>
+  </si>
+  <si>
+    <t>A3 - City</t>
+  </si>
+  <si>
+    <t>A3 - State</t>
+  </si>
+  <si>
+    <t>A3 - Zip Code</t>
+  </si>
+  <si>
+    <t>A4 - Address Line1</t>
+  </si>
+  <si>
+    <t>A4 - Address Line2</t>
+  </si>
+  <si>
+    <t>A4 - City</t>
+  </si>
+  <si>
+    <t>A4 - State</t>
+  </si>
+  <si>
+    <t>A4 - Zip Code</t>
+  </si>
+  <si>
+    <t>A5 - Address Line1</t>
+  </si>
+  <si>
+    <t>A5 - Address Line2</t>
+  </si>
+  <si>
+    <t>A5 - City</t>
+  </si>
+  <si>
+    <t>A5 - State</t>
+  </si>
+  <si>
+    <t>A5 - Zip Code</t>
+  </si>
+  <si>
+    <t>A6 - Address Line1</t>
+  </si>
+  <si>
+    <t>A6 - Address Line2</t>
+  </si>
+  <si>
+    <t>A6 - City</t>
+  </si>
+  <si>
+    <t>A6 - State</t>
+  </si>
+  <si>
+    <t>A6 - Zip Code</t>
+  </si>
+  <si>
+    <t>A7 - Address Line1</t>
+  </si>
+  <si>
+    <t>A7 - Address Line2</t>
+  </si>
+  <si>
+    <t>A7 - City</t>
+  </si>
+  <si>
+    <t>A7 - State</t>
+  </si>
+  <si>
+    <t>A7 - Zip Code</t>
+  </si>
+  <si>
+    <t>A8 - Address Line1</t>
+  </si>
+  <si>
+    <t>A8 - Address Line2</t>
+  </si>
+  <si>
+    <t>A8 - City</t>
+  </si>
+  <si>
+    <t>A8 - State</t>
+  </si>
+  <si>
+    <t>A8 - Zip Code</t>
+  </si>
+  <si>
+    <t>A9 - Address Line1</t>
+  </si>
+  <si>
+    <t>A9 - Address Line2</t>
+  </si>
+  <si>
+    <t>A9 - City</t>
+  </si>
+  <si>
+    <t>A9 - State</t>
+  </si>
+  <si>
+    <t>A9 - Zip Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         FirstName </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         LastName </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         OppName </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         FsAddress </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A1_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A1_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A1_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A1_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A1_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A2_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A2_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A2_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A2_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A2_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A3_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A3_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A3_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A3_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A3_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A4_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A4_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A4_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A4_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A4_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A5_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A5_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A5_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A5_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A5_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A6_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A6_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A6_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A6_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A6_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A7_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A7_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A7_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A7_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A7_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A8_AddressLine1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A8_AddressLine2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A8_City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A8_State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         A8_ZipCode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Template </t>
+  </si>
+  <si>
+    <t>[1.0]</t>
+  </si>
+  <si>
+    <t>[1.2]</t>
+  </si>
+  <si>
+    <t>~ add the option to print the envelope and/or the letter
+~ print in the middle of the envelop Address1 in its first line and Address2 in the second line
+~ give the user the option to generate for each contact: the letter only or envelop only or both</t>
+  </si>
+  <si>
+    <t>[1.9]</t>
+  </si>
+  <si>
+    <t>~ use the new csv format and map Apptivo template name to CDMailer template name
+~ fix: prompt for input csv incorrect
+~ zipCode: insert leading 0 if it is less than 5</t>
   </si>
 </sst>
 </file>
@@ -111,20 +402,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -151,8 +459,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="2"/>
-      <tableStyleElement type="headerRow" dxfId="1"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -167,24 +475,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:C9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Version" dataDxfId="0"/>
-    <tableColumn id="2" name="Comments"/>
-    <tableColumn id="3" name="Released"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Version"/>
-    <tableColumn id="2" name="Details"/>
-    <tableColumn id="3" name="Date"/>
+    <tableColumn id="1" name="Version" dataDxfId="3"/>
+    <tableColumn id="2" name="Details" dataDxfId="2"/>
+    <tableColumn id="3" name="Date" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -233,7 +529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,7 +564,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,68 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="49.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="93.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,49 +791,87 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C6" s="5">
+        <v>43222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C7" s="5">
+        <v>43248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3">
-        <v>43222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3">
-        <v>43248</v>
-      </c>
+      <c r="C8" s="5">
+        <v>43253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -603,4 +879,407 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[1.10] ~ Generate single contact documents
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Version</t>
   </si>
@@ -367,6 +367,12 @@
     <t>~ use the new csv format and map Apptivo template name to CDMailer template name
 ~ fix: prompt for input csv incorrect
 ~ zipCode: insert leading 0 if it is less than 5</t>
+  </si>
+  <si>
+    <t>[1.10]</t>
+  </si>
+  <si>
+    <t>~ Generate single contact documents</t>
   </si>
 </sst>
 </file>
@@ -475,12 +481,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C10"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Version" dataDxfId="3"/>
-    <tableColumn id="2" name="Details" dataDxfId="2"/>
-    <tableColumn id="3" name="Date" dataDxfId="1"/>
+    <tableColumn id="1" name="Version" dataDxfId="2"/>
+    <tableColumn id="2" name="Details" dataDxfId="1"/>
+    <tableColumn id="3" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -529,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,7 +570,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -773,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,6 +878,17 @@
         <v>113</v>
       </c>
       <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43258</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.11] ~ enable user to enter delay between documents ~ enable user to select printing method ~ enable user to select printing scope (letters/letters+envelops/envelops) ~ support PostCards
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Version</t>
   </si>
@@ -364,15 +364,25 @@
     <t>[1.9]</t>
   </si>
   <si>
+    <t>[1.10]</t>
+  </si>
+  <si>
+    <t>~ Generate single contact documents</t>
+  </si>
+  <si>
     <t>~ use the new csv format and map Apptivo template name to CDMailer template name
 ~ fix: prompt for input csv incorrect
-~ zipCode: insert leading 0 if it is less than 5</t>
-  </si>
-  <si>
-    <t>[1.10]</t>
-  </si>
-  <si>
-    <t>~ Generate single contact documents</t>
+~ zipCode: insert leading 0 if it is less than 5 digits</t>
+  </si>
+  <si>
+    <t>[1.11]</t>
+  </si>
+  <si>
+    <t>[printing]
+~ enable user to enter delay between documents
+~ enable user to select printing method
+~ enable user to select printing scope (letters/letters+envelops/envelops)
+~ support PostCards</t>
   </si>
 </sst>
 </file>
@@ -481,8 +491,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C10" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C12"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -535,7 +545,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +580,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,20 +885,36 @@
         <v>112</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="C10" s="5">
         <v>43258</v>
       </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="5">
+        <v>43275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.13] - implement postal cards - fix PC1 having extra page - use background worker for printing - fix a bug from last release that happens while generating envelops, they were not filled - implement using the same size for both envelops and postcards taken from UI
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Version</t>
   </si>
@@ -384,6 +384,17 @@
 ~ enable user to select printing scope (letters/letters+envelops/envelops)
 ~ Generate the same template for one or all contacts
 ~ support PostCards</t>
+  </si>
+  <si>
+    <t>[1.12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[printing envelops]
+- add Spire to CDMailer
+- handle case when Print is clicked without setting the output folder
+- handle envelops as size A5
+- fix a bug in filename generation for both envelops and letters
+</t>
   </si>
 </sst>
 </file>
@@ -492,8 +503,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C12" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -546,7 +557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,7 +592,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,7 +801,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -912,10 +923,21 @@
         <v>43275</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="5">
+        <v>43281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.14] - [Printing] - use the hotfix from Spire that fixes the footer issue - hide the other printing APIs options - adjust PC1 and PC2 to avoid overlapping Alberto's image when they get filled
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>Version</t>
   </si>
@@ -395,6 +395,25 @@
 - handle envelops as size A5
 - fix a bug in filename generation for both envelops and letters
 </t>
+  </si>
+  <si>
+    <t>[1.13]</t>
+  </si>
+  <si>
+    <t>[Printing]
+- implement postal cards - fix PC1 having extra page
+- use background worker for printing
+- fix a bug from last release that happens while generating envelops, they were not filled
+- implement using the same size for both envelops and postcards taken from UI</t>
+  </si>
+  <si>
+    <t>[1.14]</t>
+  </si>
+  <si>
+    <t>[Printing]
+- use the hotfix from Spire that fixes the footer issue
+- hide the other printing APIs options
+- adjust PC1 and PC2 to avoid overlapping Alberto's image when they get filled</t>
   </si>
 </sst>
 </file>
@@ -503,8 +522,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C14"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -557,7 +576,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -592,7 +611,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -801,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,15 +953,33 @@
         <v>43281</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="5">
+        <v>43283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="5">
+        <v>43304</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[1.16]  -[Printing] - customize margins for envelops - stop using landscape for envelops
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Version</t>
   </si>
@@ -414,6 +414,23 @@
 - use the hotfix from Spire that fixes the footer issue
 - hide the other printing APIs options
 - adjust PC1 and PC2 to avoid overlapping Alberto's image when they get filled</t>
+  </si>
+  <si>
+    <t>[1.15]</t>
+  </si>
+  <si>
+    <t>[Printing]
+- print on both sides for all documents by default
+- add the margins for envelops only
+- use Landscape view for envelops only</t>
+  </si>
+  <si>
+    <t>[1.16]</t>
+  </si>
+  <si>
+    <t>[Printing]
+- customize margins for envelops
+- stop using landscape for envelops</t>
   </si>
 </sst>
 </file>
@@ -522,8 +539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C16" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C16"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -576,7 +593,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,7 +628,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -820,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,6 +991,24 @@
       <c r="C14" s="5">
         <v>43304</v>
       </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.17.2] ~ separate the logic for printing envelops from printing postcards ~ use the postcards templates with white background
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Version</t>
   </si>
@@ -431,6 +431,13 @@
     <t>[Printing]
 - customize margins for envelops
 - stop using landscape for envelops</t>
+  </si>
+  <si>
+    <t>[1.17.2]</t>
+  </si>
+  <si>
+    <t>~ separate the logic for printing envelops from printing postcards
+~ use the postcards templates with white background</t>
   </si>
 </sst>
 </file>
@@ -539,8 +546,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C16" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C18" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C18"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -593,7 +600,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,7 +635,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -837,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,6 +1016,22 @@
         <v>127</v>
       </c>
       <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="5">
+        <v>43336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.17.3] ~ more robust handling for storage of int configuration values ~ more helpful logging for the case of invalid template value in the input csv
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6330"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>Version</t>
   </si>
@@ -438,6 +438,13 @@
   <si>
     <t>~ separate the logic for printing envelops from printing postcards
 ~ use the postcards templates with white background</t>
+  </si>
+  <si>
+    <t>[1.17.3]</t>
+  </si>
+  <si>
+    <t>~ more robust handling for storage of int configuration values
+~ more helpful logging for the case of invalid template value in the input csv</t>
   </si>
 </sst>
 </file>
@@ -600,7 +607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +642,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -847,7 +854,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,9 +1035,13 @@
         <v>43336</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C18" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[1.17.4] - fixed PostCard template 1 to avoid unnecessary line spaces and unnecessary breaking of the word "Government" when generated and avoid cases where Alberto's image gets displaced - making support for integer-only values for margins and page sizes (envelops and postcards) - fixed PostCard template 2 to avoid any irregular behavior while generating it
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Version</t>
   </si>
@@ -445,6 +445,14 @@
   <si>
     <t>~ more robust handling for storage of int configuration values
 ~ more helpful logging for the case of invalid template value in the input csv</t>
+  </si>
+  <si>
+    <t>[1.17.4]</t>
+  </si>
+  <si>
+    <t>~ fixed PostCard template 1 to avoid unnecessary line spaces and unnecessary breaking of the word "Government" when generated and avoid cases where Alberto's image gets displaced 
+~ making support for integer-only values for margins and page sizes (envelops and postcards)
+~ fixed PostCard template 2 to avoid any irregular behavior while generating it</t>
   </si>
 </sst>
 </file>
@@ -553,8 +561,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C18" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C19" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C19"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -851,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,6 +1051,15 @@
         <v>131</v>
       </c>
       <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.17.5] ~ adjusting Envelop template to align the recepient name at center ~ upgrading the Spire dlls to hotfix 6.8.11
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Version</t>
   </si>
@@ -453,6 +453,13 @@
     <t>~ fixed PostCard template 1 to avoid unnecessary line spaces and unnecessary breaking of the word "Government" when generated and avoid cases where Alberto's image gets displaced 
 ~ making support for integer-only values for margins and page sizes (envelops and postcards)
 ~ fixed PostCard template 2 to avoid any irregular behavior while generating it</t>
+  </si>
+  <si>
+    <t>[1.17.5]</t>
+  </si>
+  <si>
+    <t>~ adjusting Envelop template to align the recepient name at center
+~ upgrading the Spire dlls to hotfix 6.8.11</t>
   </si>
 </sst>
 </file>
@@ -561,8 +568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C19" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -859,10 +866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1060,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>132</v>
       </c>
@@ -1060,6 +1068,22 @@
         <v>133</v>
       </c>
       <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="5">
+        <v>43341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.17.7] - handle the variation of input files where we only have 5 address fields - adjust the error reported in the interface for the case of contacts with bad templates to show the First and Last names of the contacts as well as the opportunity - enable the tool to generate outputs when the custom scenario is being used, even if the contact has an invalid template assigned
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
   <si>
     <t>Version</t>
   </si>
@@ -460,6 +460,15 @@
   <si>
     <t>~ adjusting Envelop template to align the recepient name at center
 ~ upgrading the Spire dlls to hotfix 6.8.11</t>
+  </si>
+  <si>
+    <t>[1.17.7]</t>
+  </si>
+  <si>
+    <t>[handling bad templates - input file variants]
+- handle the variation of input files where we only have 5 address fields
+- adjust the error reported in the interface for the case of contacts with bad templates to show the First and Last names of the contacts as well as the opportunity
+- enable the tool to generate outputs when the custom scenario is being used, even if the contact has an invalid template assigned</t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:C21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C22"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Version" dataDxfId="2"/>
     <tableColumn id="2" name="Details" dataDxfId="1"/>
@@ -866,11 +875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18:B20"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1089,21 @@
         <v>43341</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+    <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" s="5">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[1.17.8] reads the latest template only that contains AssignedTo all the other templates that don't have it in its place will not be read. the extra columns that begin with "A1-2" will not be used in the generation since they are rare
</commit_message>
<xml_diff>
--- a/versions.xlsx
+++ b/versions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Version</t>
   </si>
@@ -469,6 +469,14 @@
 - handle the variation of input files where we only have 5 address fields
 - adjust the error reported in the interface for the case of contacts with bad templates to show the First and Last names of the contacts as well as the opportunity
 - enable the tool to generate outputs when the custom scenario is being used, even if the contact has an invalid template assigned</t>
+  </si>
+  <si>
+    <t>[1.17.8]</t>
+  </si>
+  <si>
+    <t>reads the latest template only that contains AssignedTo
+all the other templates that don't have it in its place will not be read.
+the extra columns that begin with "A1-2" will not be used in the generation since they are rare</t>
   </si>
 </sst>
 </file>
@@ -879,7 +887,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1108,16 @@
         <v>43359</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="5">
+        <v>43364</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>